<commit_message>
updated the construction and residential pages buy buttons
</commit_message>
<xml_diff>
--- a/tools/Prices/Price Worksheets.xlsx
+++ b/tools/Prices/Price Worksheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesfolk/Work/websites/dronephotography/tools/Prices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2851F61E-CE30-BC45-8CBE-9D2A0B4BE402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28CA8A7-DDE8-7040-B0A4-5F9B4EB5B19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24980" windowHeight="20940" activeTab="3" xr2:uid="{170C7173-BC3C-924D-B252-3F79CF6F2D93}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24980" windowHeight="20940" activeTab="2" xr2:uid="{170C7173-BC3C-924D-B252-3F79CF6F2D93}"/>
   </bookViews>
   <sheets>
     <sheet name="ap_services" sheetId="8" r:id="rId1"/>
@@ -399,7 +399,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
   <si>
     <t>30 Acres</t>
   </si>
@@ -477,6 +477,12 @@
   </si>
   <si>
     <t>premium</t>
+  </si>
+  <si>
+    <t>qty</t>
+  </si>
+  <si>
+    <t>price (Built: Up to 300K SF | Construction: Up to 30 Acres)</t>
   </si>
 </sst>
 </file>
@@ -535,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -545,6 +551,9 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1083,10 +1092,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3FB8BF9-B282-D74C-A298-595A3902E71F}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1095,9 +1104,11 @@
     <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="49.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1110,8 +1121,14 @@
       <c r="D1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1127,8 +1144,15 @@
         <f>'Construction Price Worksheet'!D8</f>
         <v>379.99</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="9">
+        <f>B2*G2</f>
+        <v>474.99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1144,8 +1168,16 @@
         <f>'Construction Price Worksheet'!D9</f>
         <v>762.99</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <f>SUM(G2,1)</f>
+        <v>2</v>
+      </c>
+      <c r="H3" s="9">
+        <f>B2*G3</f>
+        <v>949.98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1161,21 +1193,261 @@
         <f>'Construction Price Worksheet'!D10</f>
         <v>1114.99</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <f t="shared" ref="G4:G39" si="0">SUM(G3,1)</f>
+        <v>3</v>
+      </c>
+      <c r="H4" s="9">
+        <f>B2*G4</f>
+        <v>1424.97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H5" s="9">
+        <f>B2*G5</f>
+        <v>1899.96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H6" s="9">
+        <f>C2*G6</f>
+        <v>2134.9499999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H7" s="9">
+        <f>C2*G7</f>
+        <v>2561.94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H8" s="9">
+        <f>C2*G8</f>
+        <v>2988.9300000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H9" s="9">
+        <f>C2*G9</f>
+        <v>3415.92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H10" s="9">
+        <f>C2*G10</f>
+        <v>3842.91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H11" s="9">
+        <f>C2*G11</f>
+        <v>4269.8999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="H12" s="9">
+        <f>D2*G12</f>
+        <v>4179.8900000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H13" s="9">
+        <f>D2*G13</f>
+        <v>4559.88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="H14" s="9">
+        <f>D2*G14</f>
+        <v>4939.87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="H15" s="9">
+        <f>D2*G15</f>
+        <v>5319.8600000000006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="H16" s="9">
+        <f>D2*G16</f>
+        <v>5699.85</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="H17" s="9">
+        <f>D2*G17</f>
+        <v>6079.84</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="H18" s="9">
+        <f>D2*G18</f>
+        <v>6459.83</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="H19" s="9">
+        <f>D2*G19</f>
+        <v>6839.82</v>
+      </c>
+    </row>
+    <row r="20" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="H20" s="9">
+        <f>D2*G20</f>
+        <v>7219.81</v>
+      </c>
+    </row>
+    <row r="21" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="H21" s="9">
+        <f>D2*G21</f>
+        <v>7599.8</v>
+      </c>
+    </row>
+    <row r="22" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="H22" s="9">
+        <f>D2*G22</f>
+        <v>7979.79</v>
+      </c>
+    </row>
+    <row r="23" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="H23" s="9">
+        <f>D2*G23</f>
+        <v>8359.7800000000007</v>
+      </c>
+    </row>
+    <row r="24" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H39" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1186,7 +1458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA6E6349-9159-1A48-AAA6-32E33F5F5A35}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9:D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>